<commit_message>
Able measure PWM bits.
5465 counts = 0 (341us)
16500 counts = 1 (1030us)
</commit_message>
<xml_diff>
--- a/rf_shield/waveform.xlsx
+++ b/rf_shield/waveform.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="84" windowWidth="19008" windowHeight="8844"/>
+    <workbookView xWindow="90" yWindow="90" windowWidth="19005" windowHeight="8850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="scope_0_2" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -31,8 +32,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -514,8 +515,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -579,10 +580,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11315624387487425"/>
-          <c:y val="9.8488617270121565E-2"/>
-          <c:w val="0.86285361710151087"/>
-          <c:h val="0.88874460514611409"/>
+          <c:x val="0.11315624387487426"/>
+          <c:y val="9.8488617270121481E-2"/>
+          <c:w val="0.86285361710151132"/>
+          <c:h val="0.88874460514611431"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5978,23 +5979,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="108441600"/>
-        <c:axId val="108443136"/>
+        <c:axId val="57915648"/>
+        <c:axId val="63767680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108441600"/>
+        <c:axId val="57915648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108443136"/>
+        <c:crossAx val="63767680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108443136"/>
+        <c:axId val="63767680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6002,7 +6003,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108441600"/>
+        <c:crossAx val="57915648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6020,10 +6021,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -6345,12 +6347,12 @@
       <selection activeCell="F895" sqref="F895"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -17071,4 +17073,319 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>5465</v>
+      </c>
+      <c r="B1">
+        <f>IF(A1&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>16500</v>
+      </c>
+      <c r="B2">
+        <f>IF(A2&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>5472</v>
+      </c>
+      <c r="B3">
+        <f>IF(A3&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>5457</v>
+      </c>
+      <c r="B4">
+        <f>IF(A4&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>16483</v>
+      </c>
+      <c r="B5">
+        <f>IF(A5&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>16492</v>
+      </c>
+      <c r="B6">
+        <f>IF(A6&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>5464</v>
+      </c>
+      <c r="B7">
+        <f>IF(A7&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>16489</v>
+      </c>
+      <c r="B8">
+        <f>IF(A8&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>16486</v>
+      </c>
+      <c r="B9">
+        <f>IF(A9&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>16486</v>
+      </c>
+      <c r="B10">
+        <f>IF(A10&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>5461</v>
+      </c>
+      <c r="B11">
+        <f>IF(A11&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>16494</v>
+      </c>
+      <c r="B12">
+        <f>IF(A12&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>5470</v>
+      </c>
+      <c r="B13">
+        <f>IF(A13&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>16495</v>
+      </c>
+      <c r="B14">
+        <f>IF(A14&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>5474</v>
+      </c>
+      <c r="B15">
+        <f>IF(A15&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>5476</v>
+      </c>
+      <c r="B16">
+        <f>IF(A16&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16499</v>
+      </c>
+      <c r="B17">
+        <f>IF(A17&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>16491</v>
+      </c>
+      <c r="B18">
+        <f>IF(A18&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>16501</v>
+      </c>
+      <c r="B19">
+        <f>IF(A19&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>5469</v>
+      </c>
+      <c r="B20">
+        <f>IF(A20&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>5478</v>
+      </c>
+      <c r="B21">
+        <f>IF(A21&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>16507</v>
+      </c>
+      <c r="B22">
+        <f>IF(A22&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>5461</v>
+      </c>
+      <c r="B23">
+        <f>IF(A23&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>5469</v>
+      </c>
+      <c r="B24">
+        <f>IF(A24&gt;6000,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>12545</v>
+      </c>
+      <c r="B25">
+        <f>IF(A25&gt;6000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working with RF RX.
</commit_message>
<xml_diff>
--- a/rf_shield/waveform.xlsx
+++ b/rf_shield/waveform.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>second</t>
   </si>
@@ -25,6 +25,84 @@
   </si>
   <si>
     <t>second_zeroed</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>1 count = 500ns</t>
+  </si>
+  <si>
+    <t>sync = 10.6ms</t>
   </si>
 </sst>
 </file>
@@ -562,7 +640,58 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -581,9 +710,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.11315624387487426"/>
-          <c:y val="9.8488617270121481E-2"/>
-          <c:w val="0.86285361710151132"/>
-          <c:h val="0.88874460514611431"/>
+          <c:y val="9.8488617270121467E-2"/>
+          <c:w val="0.86285361710151154"/>
+          <c:h val="0.88874460514611442"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5979,23 +6108,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="57915648"/>
-        <c:axId val="63767680"/>
+        <c:axId val="57928320"/>
+        <c:axId val="63796736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57915648"/>
+        <c:axId val="57928320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63767680"/>
+        <c:crossAx val="63796736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63767680"/>
+        <c:axId val="63796736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6003,7 +6132,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57915648"/>
+        <c:crossAx val="57928320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6021,7 +6150,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0"/>
+    <sheetView zoomScale="145" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6341,10 +6470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C893"/>
+  <dimension ref="A1:D893"/>
   <sheetViews>
-    <sheetView topLeftCell="A879" workbookViewId="0">
-      <selection activeCell="F895" sqref="F895"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -6355,7 +6484,7 @@
     <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6366,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>4.4328800000000002E-2</v>
       </c>
@@ -6378,7 +6507,7 @@
         <v>1.31307E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>4.4380000000000003E-2</v>
       </c>
@@ -6390,7 +6519,7 @@
         <v>4.9578499999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>4.4431199999999997E-2</v>
       </c>
@@ -6402,7 +6531,7 @@
         <v>4.9980599999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>4.4482399999999998E-2</v>
       </c>
@@ -6414,7 +6543,7 @@
         <v>5.0382600000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>4.45336E-2</v>
       </c>
@@ -6426,7 +6555,7 @@
         <v>5.0382600000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2">
         <v>4.4584800000000001E-2</v>
       </c>
@@ -6438,7 +6567,7 @@
         <v>5.0784599999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>4.4636000000000002E-2</v>
       </c>
@@ -6450,7 +6579,7 @@
         <v>5.0784599999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="2">
         <v>4.4687200000000003E-2</v>
       </c>
@@ -6461,8 +6590,12 @@
       <c r="C9" s="2">
         <v>5.0784599999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="1">
+        <f>A9-A3</f>
+        <v>3.0720000000000053E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>4.4738399999999998E-2</v>
       </c>
@@ -6473,8 +6606,12 @@
       <c r="C10" s="2">
         <v>9.3532599999999994E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="1">
+        <f>A217-A10</f>
+        <v>1.0598400000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>4.4789599999999999E-2</v>
       </c>
@@ -6486,7 +6623,7 @@
         <v>5.33316E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="2">
         <v>4.48408E-2</v>
       </c>
@@ -6498,7 +6635,7 @@
         <v>5.33316E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="2">
         <v>4.4892000000000001E-2</v>
       </c>
@@ -6510,7 +6647,7 @@
         <v>1.31307E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="2">
         <v>4.4943200000000003E-2</v>
       </c>
@@ -6522,7 +6659,7 @@
         <v>1.31307E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="2">
         <v>4.4994399999999997E-2</v>
       </c>
@@ -6534,7 +6671,7 @@
         <v>-2.7070299999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" s="2">
         <v>4.5045599999999998E-2</v>
       </c>
@@ -8850,7 +8987,7 @@
         <v>-2.7070299999999999E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:4">
       <c r="A209" s="2">
         <v>5.4927200000000002E-2</v>
       </c>
@@ -8862,7 +8999,7 @@
         <v>-2.7070299999999999E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:4">
       <c r="A210" s="2">
         <v>5.4978399999999997E-2</v>
       </c>
@@ -8874,7 +9011,7 @@
         <v>-2.7070299999999999E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:4">
       <c r="A211" s="2">
         <v>5.5029599999999998E-2</v>
       </c>
@@ -8886,7 +9023,7 @@
         <v>1.31307E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:4">
       <c r="A212" s="2">
         <v>5.5080799999999999E-2</v>
       </c>
@@ -8898,7 +9035,7 @@
         <v>-2.7070299999999999E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:4">
       <c r="A213" s="2">
         <v>5.5132E-2</v>
       </c>
@@ -8910,7 +9047,7 @@
         <v>1.31307E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:4">
       <c r="A214" s="2">
         <v>5.5183200000000002E-2</v>
       </c>
@@ -8922,7 +9059,7 @@
         <v>-2.7070299999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:4">
       <c r="A215" s="2">
         <v>5.5234400000000003E-2</v>
       </c>
@@ -8934,7 +9071,7 @@
         <v>-2.7070299999999999E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:4">
       <c r="A216" s="2">
         <v>5.5285599999999997E-2</v>
       </c>
@@ -8946,7 +9083,7 @@
         <v>-2.7070299999999999E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:4">
       <c r="A217" s="2">
         <v>5.5336799999999998E-2</v>
       </c>
@@ -8958,7 +9095,7 @@
         <v>-2.7070299999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:4">
       <c r="A218" s="2">
         <v>5.5388E-2</v>
       </c>
@@ -8969,8 +9106,12 @@
       <c r="C218" s="2">
         <v>4.8774499999999996</v>
       </c>
-    </row>
-    <row r="219" spans="1:3">
+      <c r="D218" s="1">
+        <f>A237-A218</f>
+        <v>9.7280000000000283E-4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
       <c r="A219" s="2">
         <v>5.5439200000000001E-2</v>
       </c>
@@ -8982,7 +9123,7 @@
         <v>5.0382600000000002</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:4">
       <c r="A220" s="2">
         <v>5.5490400000000002E-2</v>
       </c>
@@ -8994,7 +9135,7 @@
         <v>4.9578499999999996</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:4">
       <c r="A221" s="2">
         <v>5.5541599999999997E-2</v>
       </c>
@@ -9006,7 +9147,7 @@
         <v>5.0784599999999998</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:4">
       <c r="A222" s="2">
         <v>5.5592799999999998E-2</v>
       </c>
@@ -9018,7 +9159,7 @@
         <v>5.0382600000000002</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:4">
       <c r="A223" s="2">
         <v>5.5643999999999999E-2</v>
       </c>
@@ -9030,7 +9171,7 @@
         <v>5.0382600000000002</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:4">
       <c r="A224" s="2">
         <v>5.56952E-2</v>
       </c>
@@ -17071,321 +17212,502 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C25"/>
+      <selection activeCell="B1" sqref="B1:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>5465</v>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>3</v>
       </c>
       <c r="B1">
-        <f>IF(A1&gt;6000,1,0)</f>
+        <v>2059</v>
+      </c>
+      <c r="C1">
+        <f>IF(B1&gt;1000,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <f>D1-C1</f>
         <v>0</v>
       </c>
-      <c r="C1">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>684</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C24" si="0">IF(B2&gt;1000,1,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>16500</v>
-      </c>
-      <c r="B2">
-        <f>IF(A2&gt;6000,1,0)</f>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E24" si="1">D2-C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>682</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2061</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>5472</v>
-      </c>
-      <c r="B3">
-        <f>IF(A3&gt;6000,1,0)</f>
+      <c r="E4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C3">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2061</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>5457</v>
-      </c>
-      <c r="B4">
-        <f>IF(A4&gt;6000,1,0)</f>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>684</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>16483</v>
-      </c>
-      <c r="B5">
-        <f>IF(A5&gt;6000,1,0)</f>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>2061</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>16492</v>
-      </c>
-      <c r="B6">
-        <f>IF(A6&gt;6000,1,0)</f>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>2062</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>5464</v>
-      </c>
-      <c r="B7">
-        <f>IF(A7&gt;6000,1,0)</f>
+      <c r="E8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C7">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>2063</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>16489</v>
-      </c>
-      <c r="B8">
-        <f>IF(A8&gt;6000,1,0)</f>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>683</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>2062</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>16486</v>
-      </c>
-      <c r="B9">
-        <f>IF(A9&gt;6000,1,0)</f>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>683</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>2062</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>16486</v>
-      </c>
-      <c r="B10">
-        <f>IF(A10&gt;6000,1,0)</f>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>683</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>683</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>2062</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>5461</v>
-      </c>
-      <c r="B11">
-        <f>IF(A11&gt;6000,1,0)</f>
+      <c r="E16">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C11">
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>2064</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>16494</v>
-      </c>
-      <c r="B12">
-        <f>IF(A12&gt;6000,1,0)</f>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>2060</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>5470</v>
-      </c>
-      <c r="B13">
-        <f>IF(A13&gt;6000,1,0)</f>
+      <c r="E18">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C13">
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>684</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>16495</v>
-      </c>
-      <c r="B14">
-        <f>IF(A14&gt;6000,1,0)</f>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>683</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>2062</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="D21">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>5474</v>
-      </c>
-      <c r="B15">
-        <f>IF(A15&gt;6000,1,0)</f>
+      <c r="E21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C15">
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>682</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>5476</v>
-      </c>
-      <c r="B16">
-        <f>IF(A16&gt;6000,1,0)</f>
+      <c r="D22">
         <v>0</v>
       </c>
-      <c r="C16">
+      <c r="E22">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>16499</v>
-      </c>
-      <c r="B17">
-        <f>IF(A17&gt;6000,1,0)</f>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>684</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>1540</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C17">
+      <c r="D24">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>16491</v>
-      </c>
-      <c r="B18">
-        <f>IF(A18&gt;6000,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>16501</v>
-      </c>
-      <c r="B19">
-        <f>IF(A19&gt;6000,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>5469</v>
-      </c>
-      <c r="B20">
-        <f>IF(A20&gt;6000,1,0)</f>
+      <c r="E24">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>5478</v>
-      </c>
-      <c r="B21">
-        <f>IF(A21&gt;6000,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>16507</v>
-      </c>
-      <c r="B22">
-        <f>IF(A22&gt;6000,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>5461</v>
-      </c>
-      <c r="B23">
-        <f>IF(A23&gt;6000,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>5469</v>
-      </c>
-      <c r="B24">
-        <f>IF(A24&gt;6000,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25">
-        <v>12545</v>
-      </c>
-      <c r="B25">
-        <f>IF(A25&gt;6000,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>